<commit_message>
Write XML to new file working. Ready for more fields
</commit_message>
<xml_diff>
--- a/comet_api_example/File Specification - Update_3.26.18.xlsx
+++ b/comet_api_example/File Specification - Update_3.26.18.xlsx
@@ -1,33 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Research\Paustian\CFARM\api\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/comet_api_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5A3F4C-0C07-41B1-92DF-15734C0983A3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F49D3BF-4190-5043-9A7B-ED6515F0AC47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22400" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input File" sheetId="5" r:id="rId1"/>
     <sheet name="Results File" sheetId="2" r:id="rId2"/>
     <sheet name="Units" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="Crops">Units!$A$2:$A$34</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="272">
   <si>
     <t>&lt;Day cometEmailId="mark.easter@colostate.edu"&gt;</t>
   </si>
@@ -828,13 +839,28 @@
   </si>
   <si>
     <t>&lt;CropYear definitions repeat for each year from 2000 to the current calendar year - 1&gt;</t>
+  </si>
+  <si>
+    <t>Crop</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>dpollard@ecotrust.org</t>
+  </si>
+  <si>
+    <t>CRP</t>
+  </si>
+  <si>
+    <t>No'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -854,6 +880,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -926,11 +960,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -938,9 +973,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1256,36 +1294,36 @@
   <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="69.5" customWidth="1"/>
     <col min="8" max="8" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>100</v>
       </c>
@@ -1299,7 +1337,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>101</v>
       </c>
@@ -1313,7 +1351,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>102</v>
       </c>
@@ -1327,7 +1365,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>103</v>
       </c>
@@ -1341,7 +1379,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>104</v>
       </c>
@@ -1355,7 +1393,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>156</v>
       </c>
@@ -1369,7 +1407,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>157</v>
       </c>
@@ -1383,7 +1421,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>158</v>
       </c>
@@ -1397,7 +1435,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>159</v>
       </c>
@@ -1411,7 +1449,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>105</v>
       </c>
@@ -1425,7 +1463,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>106</v>
       </c>
@@ -1439,7 +1477,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>107</v>
       </c>
@@ -1451,7 +1489,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>108</v>
@@ -1463,7 +1501,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
@@ -1477,7 +1515,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1491,7 +1529,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1505,7 +1543,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1519,7 +1557,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1533,7 +1571,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1547,7 +1585,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1559,7 +1597,7 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1571,7 +1609,7 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1585,7 +1623,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1599,7 +1637,7 @@
       </c>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1613,7 +1651,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1627,7 +1665,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1639,7 +1677,7 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1651,7 +1689,7 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1663,7 +1701,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1675,7 +1713,7 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1687,7 +1725,7 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1699,7 +1737,7 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1713,7 +1751,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1727,7 +1765,7 @@
       </c>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1739,7 +1777,7 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1751,7 +1789,7 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1763,7 +1801,7 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1775,7 +1813,7 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1789,7 +1827,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1803,7 +1841,7 @@
       </c>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1817,7 +1855,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1831,7 +1869,7 @@
       </c>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -1845,7 +1883,7 @@
       </c>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -1857,7 +1895,7 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -1869,7 +1907,7 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1881,7 +1919,7 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -1893,7 +1931,7 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -1907,7 +1945,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1921,7 +1959,7 @@
       </c>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -1935,7 +1973,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -1949,7 +1987,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -1961,7 +1999,7 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -1973,7 +2011,7 @@
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -1985,7 +2023,7 @@
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -1997,7 +2035,7 @@
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -2009,7 +2047,7 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -2023,7 +2061,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -2037,7 +2075,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -2049,7 +2087,7 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2061,7 +2099,7 @@
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
     </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -2073,7 +2111,7 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -2085,7 +2123,7 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
     </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -2099,7 +2137,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -2113,7 +2151,7 @@
       </c>
       <c r="J66" s="4"/>
     </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -2127,7 +2165,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2139,7 +2177,7 @@
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
     </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -2151,7 +2189,7 @@
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
     </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -2163,7 +2201,7 @@
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -2175,7 +2213,7 @@
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
     </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -2189,7 +2227,7 @@
       </c>
       <c r="J72" s="4"/>
     </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -2201,7 +2239,7 @@
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
     </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -2213,7 +2251,7 @@
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="s">
@@ -2225,7 +2263,7 @@
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
@@ -2239,7 +2277,7 @@
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2251,7 +2289,7 @@
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -2263,7 +2301,7 @@
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="s">
@@ -2275,7 +2313,7 @@
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
         <v>143</v>
@@ -2287,7 +2325,7 @@
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
         <v>266</v>
@@ -2299,7 +2337,7 @@
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C82" s="1" t="s">
         <v>144</v>
       </c>
@@ -2311,12 +2349,12 @@
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -2330,513 +2368,511 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:XFD135"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F42" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F49" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F50" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F51" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F53" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F54" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F55" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F56" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F57" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F58" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F59" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E60" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D61" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D62" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E63" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F64" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F65" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F66" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F67" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F68" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F69" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F70" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E71" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E72" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F73" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F74" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F75" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F76" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F77" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F78" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E79" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E80" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F81" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F82" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F83" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F84" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F85" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F86" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F87" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F88" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E89" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E90" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F91" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F92" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F93" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F94" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F95" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F96" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E97" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D98" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>1</v>
       </c>
@@ -2850,17 +2886,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView showWhiteSpace="0" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>151</v>
       </c>
@@ -2868,7 +2905,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -2876,7 +2913,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -2884,7 +2921,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>172</v>
       </c>
@@ -2892,7 +2929,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -2900,7 +2937,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -2908,7 +2945,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>176</v>
       </c>
@@ -2916,7 +2953,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>177</v>
       </c>
@@ -2924,7 +2961,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -2932,7 +2969,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -2940,7 +2977,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>180</v>
       </c>
@@ -2948,7 +2985,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>181</v>
       </c>
@@ -2956,7 +2993,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>182</v>
       </c>
@@ -2964,7 +3001,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>183</v>
       </c>
@@ -2972,7 +3009,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -2980,7 +3017,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -2988,7 +3025,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>186</v>
       </c>
@@ -2996,7 +3033,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>187</v>
       </c>
@@ -3004,7 +3041,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>188</v>
       </c>
@@ -3012,7 +3049,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>189</v>
       </c>
@@ -3020,7 +3057,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>190</v>
       </c>
@@ -3028,7 +3065,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -3036,7 +3073,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>192</v>
       </c>
@@ -3044,7 +3081,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>193</v>
       </c>
@@ -3052,7 +3089,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>194</v>
       </c>
@@ -3060,7 +3097,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>195</v>
       </c>
@@ -3068,7 +3105,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>196</v>
       </c>
@@ -3076,7 +3113,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>197</v>
       </c>
@@ -3084,7 +3121,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>198</v>
       </c>
@@ -3092,7 +3129,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>199</v>
       </c>
@@ -3100,7 +3137,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>200</v>
       </c>
@@ -3108,7 +3145,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>201</v>
       </c>
@@ -3116,7 +3153,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>202</v>
       </c>
@@ -3124,7 +3161,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>203</v>
       </c>
@@ -3132,7 +3169,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>259</v>
       </c>
@@ -3140,7 +3177,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>204</v>
       </c>
@@ -3148,7 +3185,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>204</v>
       </c>
@@ -3156,7 +3193,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>205</v>
       </c>
@@ -3164,7 +3201,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>206</v>
       </c>
@@ -3172,7 +3209,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>176</v>
       </c>
@@ -3180,7 +3217,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>177</v>
       </c>
@@ -3188,7 +3225,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>207</v>
       </c>
@@ -3196,7 +3233,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>187</v>
       </c>
@@ -3204,7 +3241,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -3212,7 +3249,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>209</v>
       </c>
@@ -3220,7 +3257,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>193</v>
       </c>
@@ -3228,7 +3265,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>210</v>
       </c>
@@ -3236,7 +3273,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>203</v>
       </c>
@@ -3244,7 +3281,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>260</v>
       </c>
@@ -3252,72 +3289,129 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>223</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{66361A7E-3A19-5545-B474-112BA9254CF5}">
+      <formula1>Crops</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFC02AB-C1C2-B949-BB90-785BB2B0FDCF}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="1" workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Choose a crop" error="Choose a crop" sqref="B2" xr:uid="{3E54C216-C15D-5E46-806E-D9B1717DFD99}">
+      <formula1>Crops</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{66D3FC59-16BF-BE46-9961-CC1B8614A333}">
+      <formula1>"'Yes', 'No'"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{9CE42193-6934-5440-8E67-898B8A653301}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>